<commit_message>
translate back to Chinese
</commit_message>
<xml_diff>
--- a/distraction_prompts.xlsx
+++ b/distraction_prompts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b442eee93064521/Documents/TMS_EEG_project/RST_alpha/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chenxiao/Documents/project_codes/RST_Chinese_beta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{30F20ADF-6F92-2341-A428-05A51FD99FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91C4A1F1-8987-5749-A386-ACFDEDF0020C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBE04C1-9B4F-A848-8F52-9A788869DE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{6E9AD0D5-BB09-ED4E-A686-B1F490344749}"/>
+    <workbookView xWindow="15380" yWindow="1020" windowWidth="27640" windowHeight="16940" xr2:uid="{6E9AD0D5-BB09-ED4E-A686-B1F490344749}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,16 +44,16 @@
     <t>prompt</t>
   </si>
   <si>
-    <t>The layout of a typical classroom</t>
-  </si>
-  <si>
-    <t>Raindrops sliding down a windowpane</t>
-  </si>
-  <si>
-    <t>Clouds forming in the sky</t>
-  </si>
-  <si>
-    <t>A train stopped at a station</t>
+    <t>一间教室的典型布置</t>
+  </si>
+  <si>
+    <t>窗户上雨滴顺着玻璃滑下</t>
+  </si>
+  <si>
+    <t>天空中布满云朵</t>
+  </si>
+  <si>
+    <t>火车停在火车站的情形</t>
   </si>
 </sst>
 </file>
@@ -106,10 +106,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>